<commit_message>
budget_tables_draft2017b.ipynb: changing order of column in Tables 4 and S4
</commit_message>
<xml_diff>
--- a/analysis_draft2017b/csv/tS04.xlsx
+++ b/analysis_draft2017b/csv/tS04.xlsx
@@ -16,12 +16,12 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
   <si>
+    <t>Sea salt aerosol</t>
+  </si>
+  <si>
     <t>Dust aerosol</t>
   </si>
   <si>
-    <t>Sea salt aerosol</t>
-  </si>
-  <si>
     <t>Sources, Tg/yr</t>
   </si>
   <si>
@@ -43,6 +43,24 @@
     <t>Lifetime, days</t>
   </si>
   <si>
+    <t>+5510.06 ± 14.81</t>
+  </si>
+  <si>
+    <t>-5559.09 ± 14.96</t>
+  </si>
+  <si>
+    <t>-2327.11 ± 5.73</t>
+  </si>
+  <si>
+    <t>-3231.97 ± 9.45</t>
+  </si>
+  <si>
+    <t>+9.66 ± 0.02</t>
+  </si>
+  <si>
+    <t>+0.63 ± 0.00</t>
+  </si>
+  <si>
     <t>+3789.26 ± 21.87</t>
   </si>
   <si>
@@ -59,24 +77,6 @@
   </si>
   <si>
     <t>+4.00 ± 0.03</t>
-  </si>
-  <si>
-    <t>+5510.06 ± 14.81</t>
-  </si>
-  <si>
-    <t>-5559.09 ± 14.96</t>
-  </si>
-  <si>
-    <t>-2327.11 ± 5.73</t>
-  </si>
-  <si>
-    <t>-3231.97 ± 9.45</t>
-  </si>
-  <si>
-    <t>+9.66 ± 0.02</t>
-  </si>
-  <si>
-    <t>+0.63 ± 0.00</t>
   </si>
 </sst>
 </file>

</xml_diff>